<commit_message>
Added switchable controller/peripheral mode
</commit_message>
<xml_diff>
--- a/teensy4_1_pin_assignments.xlsx
+++ b/teensy4_1_pin_assignments.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkd\Documents\projects\2022\pertec_arduino_adapter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A62E40-9E30-4D3A-AD2A-247124067753}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E2B8D6-7897-4837-A384-F457D50A6D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5430" yWindow="2655" windowWidth="19515" windowHeight="11835" xr2:uid="{D47DA262-0BB6-41A9-A122-1FE01831C68C}"/>
-    <workbookView xWindow="8970" yWindow="3075" windowWidth="19515" windowHeight="11835" activeTab="2" xr2:uid="{72A8A54D-C743-4A12-96C0-ED0694AD2EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="TeensyPinAssignments" sheetId="1" r:id="rId1"/>
@@ -5682,10 +5681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2419A856-84D9-42CE-9B99-8593675AE48D}">
   <dimension ref="A1:M176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K62" sqref="K62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K61" sqref="K61"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11477,7 +11475,6 @@
   <dimension ref="A1:M204"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18257,9 +18254,6 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="1">
-      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20273,7 +20267,6 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20382,7 +20375,6 @@
     <sheetView topLeftCell="A291" workbookViewId="0">
       <selection activeCell="B317" sqref="B317"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Development checkpoint: ready to start layout
</commit_message>
<xml_diff>
--- a/teensy4_1_pin_assignments.xlsx
+++ b/teensy4_1_pin_assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkd\Documents\projects\2022\pertec_arduino_adapter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E2B8D6-7897-4837-A384-F457D50A6D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3589F640-034B-4CBE-8A51-7B23B9CC3628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="2655" windowWidth="19515" windowHeight="11835" xr2:uid="{D47DA262-0BB6-41A9-A122-1FE01831C68C}"/>
+    <workbookView xWindow="9735" yWindow="2550" windowWidth="19515" windowHeight="11835" xr2:uid="{D47DA262-0BB6-41A9-A122-1FE01831C68C}"/>
   </bookViews>
   <sheets>
     <sheet name="TeensyPinAssignments" sheetId="1" r:id="rId1"/>
@@ -5191,13 +5191,13 @@
     <t>LSOE</t>
   </si>
   <si>
-    <t>LSDIRA</t>
-  </si>
-  <si>
     <t>LSDIRB</t>
   </si>
   <si>
     <t>LPI2C4_INT</t>
+  </si>
+  <si>
+    <t>DIRA</t>
   </si>
 </sst>
 </file>
@@ -5681,8 +5681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2419A856-84D9-42CE-9B99-8593675AE48D}">
   <dimension ref="A1:M176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7498,7 +7498,7 @@
         <v>3</v>
       </c>
       <c r="K59" t="s">
-        <v>1719</v>
+        <v>1721</v>
       </c>
       <c r="L59" s="3" t="str">
         <f>IFERROR(CONCATENATE(INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),5),":",INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),6)),"")</f>
@@ -7578,7 +7578,7 @@
         <v>5</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="L61" s="3" t="str">
         <f>IFERROR(CONCATENATE(INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),5),":",INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),6)),"")</f>
@@ -8058,7 +8058,7 @@
         <v>28</v>
       </c>
       <c r="K73" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="L73" s="3" t="str">
         <f>IFERROR(CONCATENATE(INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),5),":",INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),6)),"")</f>

</xml_diff>

<commit_message>
Corrected names of OEA and DIRA/DIRB signals
</commit_message>
<xml_diff>
--- a/teensy4_1_pin_assignments.xlsx
+++ b/teensy4_1_pin_assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkd\Documents\projects\2022\pertec_arduino_adapter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3589F640-034B-4CBE-8A51-7B23B9CC3628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB6D640-AF2B-42D3-BDC0-1C4595E762CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9735" yWindow="2550" windowWidth="19515" windowHeight="11835" xr2:uid="{D47DA262-0BB6-41A9-A122-1FE01831C68C}"/>
+    <workbookView xWindow="5430" yWindow="2265" windowWidth="19290" windowHeight="12810" xr2:uid="{D47DA262-0BB6-41A9-A122-1FE01831C68C}"/>
   </bookViews>
   <sheets>
     <sheet name="TeensyPinAssignments" sheetId="1" r:id="rId1"/>
@@ -5188,16 +5188,16 @@
     <t>Pinname</t>
   </si>
   <si>
-    <t>LSOE</t>
-  </si>
-  <si>
-    <t>LSDIRB</t>
-  </si>
-  <si>
     <t>LPI2C4_INT</t>
   </si>
   <si>
     <t>DIRA</t>
+  </si>
+  <si>
+    <t>DIRB</t>
+  </si>
+  <si>
+    <t>OEA</t>
   </si>
 </sst>
 </file>
@@ -5681,8 +5681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2419A856-84D9-42CE-9B99-8593675AE48D}">
   <dimension ref="A1:M176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7498,7 +7498,7 @@
         <v>3</v>
       </c>
       <c r="K59" t="s">
-        <v>1721</v>
+        <v>1719</v>
       </c>
       <c r="L59" s="3" t="str">
         <f>IFERROR(CONCATENATE(INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),5),":",INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),6)),"")</f>
@@ -7578,7 +7578,7 @@
         <v>5</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
       <c r="L61" s="3" t="str">
         <f>IFERROR(CONCATENATE(INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),5),":",INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),6)),"")</f>
@@ -8058,7 +8058,7 @@
         <v>28</v>
       </c>
       <c r="K73" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="L73" s="3" t="str">
         <f>IFERROR(CONCATENATE(INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),5),":",INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),6)),"")</f>
@@ -8098,7 +8098,7 @@
         <v>29</v>
       </c>
       <c r="K74" t="s">
-        <v>1718</v>
+        <v>1721</v>
       </c>
       <c r="L74" s="3" t="str">
         <f>IFERROR(CONCATENATE(INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),5),":",INDEX(PertecSignals[],MATCH(TeensyPinTable[[#This Row],[My Design]],PertecSignals[Signal Name],0),6)),"")</f>

</xml_diff>